<commit_message>
Update RFCN Mini Drone Results
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Average Precision</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Network</t>
   </si>
   <si>
-    <t>DataSet</t>
-  </si>
-  <si>
     <t>Training Dataset</t>
   </si>
   <si>
@@ -63,13 +60,22 @@
   </si>
   <si>
     <t>False Negative</t>
+  </si>
+  <si>
+    <t>Atul Gupta</t>
+  </si>
+  <si>
+    <t>RFCN</t>
+  </si>
+  <si>
+    <t>Mini Drone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +85,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -124,18 +137,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F2" sqref="F2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,19 +445,18 @@
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -456,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>10</v>
@@ -465,34 +485,57 @@
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3">
+        <v>15347</v>
+      </c>
+      <c r="H2" s="3">
+        <v>26931</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <f>G2/(G2+H2)</f>
+        <v>0.36300203415487958</v>
+      </c>
+      <c r="K2" s="4">
+        <f>H2/(H2+I2)</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="4">
+        <f>2*(J2*K2)/(J2+K2)</f>
+        <v>0.53265075921908889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -505,9 +548,8 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -520,9 +562,8 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -535,9 +576,8 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -550,9 +590,8 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -565,9 +604,8 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -580,7 +618,6 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
VOC 2 class Train results
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\ACVI2018\person-detection\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chandra\Personal\lessons\Data Science\IITH\Class\Advanced Machine Learning\Project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Average Precision</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Mini Drone</t>
+  </si>
+  <si>
+    <t>Chandra</t>
+  </si>
+  <si>
+    <t>Faster RCNN</t>
+  </si>
+  <si>
+    <t>VOC 2C</t>
   </si>
 </sst>
 </file>
@@ -437,26 +446,26 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:L2"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -494,7 +503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -535,35 +544,89 @@
         <v>0.53265075921908889</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4368</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3264</v>
+      </c>
+      <c r="I3" s="1">
+        <v>24002</v>
+      </c>
+      <c r="J3" s="4">
+        <f>G3/(G3+H3)</f>
+        <v>0.57232704402515722</v>
+      </c>
+      <c r="K3" s="4">
+        <f>H3/(H3+I3)</f>
+        <v>0.11970952835032642</v>
+      </c>
+      <c r="L3" s="4">
+        <f>2*(J3*K3)/(J3+K3)</f>
+        <v>0.19800398775807598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12120</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10769</v>
+      </c>
+      <c r="I4" s="1">
+        <v>31589</v>
+      </c>
+      <c r="J4" s="4">
+        <f>G4/(G4+H4)</f>
+        <v>0.52951199266022986</v>
+      </c>
+      <c r="K4" s="4">
+        <f>H4/(H4+I4)</f>
+        <v>0.25423768827612259</v>
+      </c>
+      <c r="L4" s="4">
+        <f>2*(J4*K4)/(J4+K4)</f>
+        <v>0.34353291159898419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -577,7 +640,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -591,7 +654,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -605,7 +668,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>

</xml_diff>

<commit_message>
updated Okutama new results
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
   <si>
     <t>Sr. No</t>
   </si>
@@ -486,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,7 +788,7 @@
         <v>0.11970952835032642</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" ref="N7:N18" si="2">2*(L7*M7)/(L7+M7)</f>
+        <f t="shared" ref="N7:N19" si="2">2*(L7*M7)/(L7+M7)</f>
         <v>0.19800398775807598</v>
       </c>
     </row>
@@ -909,11 +909,11 @@
         <v>1734</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ref="L10" si="3">I10/(I10+J10)</f>
+        <f t="shared" ref="L10:L11" si="3">I10/(I10+J10)</f>
         <v>0.5202090125496851</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" ref="M10" si="4">J10/(J10+K10)</f>
+        <f t="shared" ref="M10:M11" si="4">J10/(J10+K10)</f>
         <v>0.8610242846838182</v>
       </c>
       <c r="N10" s="4">
@@ -925,35 +925,43 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="7">
         <v>100000</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4">
-        <v>0.90286054827175199</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0.60855593492669202</v>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7">
+        <v>24656</v>
+      </c>
+      <c r="J11" s="7">
+        <v>38849</v>
+      </c>
+      <c r="K11" s="7">
+        <v>25549</v>
+      </c>
+      <c r="L11" s="8">
+        <f t="shared" si="3"/>
+        <v>0.38825289347295489</v>
+      </c>
+      <c r="M11" s="8">
+        <f t="shared" si="4"/>
+        <v>0.60326407652411562</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.72705458908218346</v>
+        <f t="shared" ref="N11" si="5">2*(L11*M11)/(L11+M11)</f>
+        <v>0.47244581853091222</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -970,7 +978,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3">
         <v>100000</v>
@@ -981,14 +989,14 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="4">
-        <v>0.61512791991101201</v>
+        <v>0.90286054827175199</v>
       </c>
       <c r="M12" s="4">
-        <v>5.5275126193213099E-2</v>
+        <v>0.60855593492669202</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="2"/>
-        <v>0.10143531893428723</v>
+        <v>0.72705458908218346</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1005,7 +1013,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F13" s="3">
         <v>100000</v>
@@ -1016,14 +1024,14 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="4">
-        <v>0.36324786324786301</v>
+        <v>0.61512791991101201</v>
       </c>
       <c r="M13" s="4">
-        <v>8.8529678272733904E-4</v>
+        <v>5.5275126193213099E-2</v>
       </c>
       <c r="N13" s="4">
         <f t="shared" si="2"/>
-        <v>1.7662888193917732E-3</v>
+        <v>0.10143531893428723</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1037,13 +1045,13 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
@@ -1051,14 +1059,14 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="4">
-        <v>0.81307222787385602</v>
+        <v>0.36324786324786301</v>
       </c>
       <c r="M14" s="4">
-        <v>0.33167341010478302</v>
+        <v>8.8529678272733904E-4</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="2"/>
-        <v>0.47115172058065036</v>
+        <v>1.7662888193917732E-3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1066,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
@@ -1078,7 +1086,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="4"/>
@@ -1086,14 +1094,14 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="4">
-        <v>0.81679999999999997</v>
+        <v>0.81307222787385602</v>
       </c>
       <c r="M15" s="4">
-        <v>0.32529999999999998</v>
+        <v>0.33167341010478302</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="2"/>
-        <v>0.46529207600035016</v>
+        <v>0.47115172058065036</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1110,7 +1118,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F16" s="3">
         <v>60000</v>
@@ -1121,14 +1129,14 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="4">
-        <v>0.39679999999999999</v>
+        <v>0.81679999999999997</v>
       </c>
       <c r="M16" s="4">
-        <v>1.2E-2</v>
+        <v>0.32529999999999998</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" si="2"/>
-        <v>2.3295499021526417E-2</v>
+        <v>0.46529207600035016</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1136,19 +1144,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="3">
-        <v>10000</v>
+        <v>60000</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
@@ -1156,14 +1164,14 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="4">
-        <v>0.875</v>
+        <v>0.39679999999999999</v>
       </c>
       <c r="M17" s="4">
-        <v>1.3760000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="N17" s="4">
         <f t="shared" si="2"/>
-        <v>2.747679078386446E-3</v>
+        <v>2.3295499021526417E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1171,19 +1179,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>24</v>
+      <c r="F18" s="3">
+        <v>10000</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
@@ -1191,14 +1199,14 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="4">
-        <v>0.77470000000000006</v>
+        <v>0.875</v>
       </c>
       <c r="M18" s="4">
-        <v>2E-3</v>
+        <v>1.3760000000000001E-3</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="2"/>
-        <v>3.9897000128749837E-3</v>
+        <v>2.747679078386446E-3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1212,13 +1220,13 @@
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
@@ -1226,14 +1234,14 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="4">
-        <v>0.86809999999999998</v>
+        <v>0.77470000000000006</v>
       </c>
       <c r="M19" s="4">
-        <v>2.588E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="N19" s="4">
-        <f t="shared" ref="N19" si="5">2*(L19*M19)/(L19+M19)</f>
-        <v>5.1606150538424786E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.9897000128749837E-3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1247,13 +1255,13 @@
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
@@ -1261,31 +1269,50 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="4">
-        <v>0.88690000000000002</v>
+        <v>0.86809999999999998</v>
       </c>
       <c r="M20" s="4">
-        <v>3.0850000000000001E-3</v>
+        <v>2.588E-3</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" ref="N20" si="6">2*(L20*M20)/(L20+M20)</f>
-        <v>6.1486126170665796E-3</v>
+        <v>5.1606150538424786E-3</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
+      <c r="L21" s="4">
+        <v>0.88690000000000002</v>
+      </c>
+      <c r="M21" s="4">
+        <v>3.0850000000000001E-3</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" ref="N21" si="7">2*(L21*M21)/(L21+M21)</f>
+        <v>6.1486126170665796E-3</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -1351,9 +1378,25 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:M15">
-    <sortCondition ref="B2:B15"/>
+  <sortState ref="A2:M16">
+    <sortCondition ref="B2:B16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>